<commit_message>
update log off and layout
</commit_message>
<xml_diff>
--- a/WebReport/WebReport/Content/upload/bao cao choi.xlsx
+++ b/WebReport/WebReport/Content/upload/bao cao choi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zawsz\OneDrive\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA136CEC-287F-4021-8901-B3D800316912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFD3CDD-AC92-4E33-AAF6-6A2AB8C3E439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D8E16A41-8E87-4CCF-B28E-281DB6006C9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D8E16A41-8E87-4CCF-B28E-281DB6006C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>TT</t>
   </si>
@@ -567,6 +559,12 @@
   </si>
   <si>
     <t>CHITIEU</t>
+  </si>
+  <si>
+    <t>TLQUY</t>
+  </si>
+  <si>
+    <t>TLNAM</t>
   </si>
 </sst>
 </file>
@@ -574,21 +572,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_)_$_ ;_ * \(#,##0\)_$_ ;_ * &quot;-&quot;??_)_$_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -653,7 +651,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -985,25 +983,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF96DBDC-24BE-4021-B36F-6A433E65D793}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.75" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
-    <col min="5" max="5" width="20.875" customWidth="1"/>
-    <col min="6" max="6" width="21.25" customWidth="1"/>
-    <col min="7" max="7" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1020,16 +1020,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1054,8 +1060,14 @@
       <c r="H2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1080,8 +1092,14 @@
       <c r="H3" s="5">
         <v>28897000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I3" s="5">
+        <v>28897000000</v>
+      </c>
+      <c r="J3" s="5">
+        <v>28897000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1106,8 +1124,14 @@
       <c r="H4" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1132,8 +1156,14 @@
       <c r="H5" s="5">
         <v>20153000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I5" s="5">
+        <v>20153000000</v>
+      </c>
+      <c r="J5" s="5">
+        <v>20153000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1158,8 +1188,14 @@
       <c r="H6" s="5">
         <v>8744000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I6" s="5">
+        <v>8744000000</v>
+      </c>
+      <c r="J6" s="5">
+        <v>8744000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1184,8 +1220,14 @@
       <c r="H7" s="5">
         <v>14018000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I7" s="5">
+        <v>14018000000</v>
+      </c>
+      <c r="J7" s="5">
+        <v>14018000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1210,8 +1252,14 @@
       <c r="H8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1236,8 +1284,14 @@
       <c r="H9" s="5">
         <v>14018000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I9" s="5">
+        <v>14018000000</v>
+      </c>
+      <c r="J9" s="5">
+        <v>14018000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1262,8 +1316,14 @@
       <c r="H10" s="5">
         <v>9988000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I10" s="5">
+        <v>9988000000</v>
+      </c>
+      <c r="J10" s="5">
+        <v>9988000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1288,8 +1348,14 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -1314,8 +1380,14 @@
       <c r="H12" s="5">
         <v>9988000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I12" s="5">
+        <v>9988000000</v>
+      </c>
+      <c r="J12" s="5">
+        <v>9988000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1340,8 +1412,14 @@
       <c r="H13" s="5">
         <v>8370000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I13" s="5">
+        <v>8370000000</v>
+      </c>
+      <c r="J13" s="5">
+        <v>8370000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1366,8 +1444,14 @@
       <c r="H14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1392,8 +1476,14 @@
       <c r="H15" s="5">
         <v>8370000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I15" s="5">
+        <v>8370000000</v>
+      </c>
+      <c r="J15" s="5">
+        <v>8370000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1418,8 +1508,14 @@
       <c r="H16" s="5">
         <v>14200000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I16" s="5">
+        <v>14200000000</v>
+      </c>
+      <c r="J16" s="5">
+        <v>14200000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1444,8 +1540,14 @@
       <c r="H17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1470,8 +1572,14 @@
       <c r="H18" s="5">
         <v>10898000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I18" s="5">
+        <v>10898000000</v>
+      </c>
+      <c r="J18" s="5">
+        <v>10898000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1496,8 +1604,14 @@
       <c r="H19" s="5">
         <v>3302000000</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I19" s="5">
+        <v>3302000000</v>
+      </c>
+      <c r="J19" s="5">
+        <v>3302000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1522,8 +1636,14 @@
       <c r="H20" s="5">
         <v>12475000000</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I20" s="5">
+        <v>12475000000</v>
+      </c>
+      <c r="J20" s="5">
+        <v>12475000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1548,8 +1668,14 @@
       <c r="H21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1574,8 +1700,14 @@
       <c r="H22" s="5">
         <v>6453000000</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I22" s="5">
+        <v>6453000000</v>
+      </c>
+      <c r="J22" s="5">
+        <v>6453000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1600,8 +1732,14 @@
       <c r="H23" s="5">
         <v>6022000000</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I23" s="5">
+        <v>6022000000</v>
+      </c>
+      <c r="J23" s="5">
+        <v>6022000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1626,8 +1764,14 @@
       <c r="H24" s="5">
         <v>11363000000</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I24" s="5">
+        <v>11363000000</v>
+      </c>
+      <c r="J24" s="5">
+        <v>11363000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1652,8 +1796,14 @@
       <c r="H25" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1678,8 +1828,14 @@
       <c r="H26" s="5">
         <v>11363000000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I26" s="5">
+        <v>11363000000</v>
+      </c>
+      <c r="J26" s="5">
+        <v>11363000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1704,8 +1860,14 @@
       <c r="H27" s="5">
         <v>16600000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I27" s="5">
+        <v>16600000000</v>
+      </c>
+      <c r="J27" s="5">
+        <v>16600000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1730,8 +1892,14 @@
       <c r="H28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1756,8 +1924,14 @@
       <c r="H29" s="5">
         <v>9526000000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I29" s="5">
+        <v>9526000000</v>
+      </c>
+      <c r="J29" s="5">
+        <v>9526000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1782,8 +1956,14 @@
       <c r="H30" s="5">
         <v>7074000000</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I30" s="5">
+        <v>7074000000</v>
+      </c>
+      <c r="J30" s="5">
+        <v>7074000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1808,8 +1988,14 @@
       <c r="H31" s="5">
         <v>13609000000</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I31" s="5">
+        <v>13609000000</v>
+      </c>
+      <c r="J31" s="5">
+        <v>13609000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1834,8 +2020,14 @@
       <c r="H32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -1860,8 +2052,14 @@
       <c r="H33" s="5">
         <v>13609000000</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I33" s="5">
+        <v>13609000000</v>
+      </c>
+      <c r="J33" s="5">
+        <v>13609000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -1886,8 +2084,14 @@
       <c r="H34" s="5">
         <v>9497000000</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I34" s="5">
+        <v>9497000000</v>
+      </c>
+      <c r="J34" s="5">
+        <v>9497000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1912,8 +2116,14 @@
       <c r="H35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1938,8 +2148,14 @@
       <c r="H36" s="5">
         <v>9497000000</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I36" s="5">
+        <v>9497000000</v>
+      </c>
+      <c r="J36" s="5">
+        <v>9497000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1964,8 +2180,14 @@
       <c r="H37" s="5">
         <v>10590000000</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I37" s="5">
+        <v>10590000000</v>
+      </c>
+      <c r="J37" s="5">
+        <v>10590000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1990,8 +2212,14 @@
       <c r="H38" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -2016,8 +2244,14 @@
       <c r="H39" s="5">
         <v>5764000000</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I39" s="5">
+        <v>5764000000</v>
+      </c>
+      <c r="J39" s="5">
+        <v>5764000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -2042,8 +2276,14 @@
       <c r="H40" s="5">
         <v>4826000000</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I40" s="5">
+        <v>4826000000</v>
+      </c>
+      <c r="J40" s="5">
+        <v>4826000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -2068,8 +2308,14 @@
       <c r="H41" s="5">
         <v>1471700000000</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I41" s="5">
+        <v>1471700000000</v>
+      </c>
+      <c r="J41" s="5">
+        <v>1471700000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>43</v>
       </c>
@@ -2094,8 +2340,14 @@
       <c r="H42" s="5">
         <v>291188000000</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I42" s="5">
+        <v>291188000000</v>
+      </c>
+      <c r="J42" s="5">
+        <v>291188000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>45</v>
       </c>
@@ -2120,8 +2372,14 @@
       <c r="H43" s="5">
         <v>29700000000</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I43" s="5">
+        <v>29700000000</v>
+      </c>
+      <c r="J43" s="5">
+        <v>29700000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>46</v>
       </c>
@@ -2146,8 +2404,14 @@
       <c r="H44" s="5">
         <v>31000000000</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I44" s="5">
+        <v>31000000000</v>
+      </c>
+      <c r="J44" s="5">
+        <v>31000000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>47</v>
       </c>
@@ -2172,8 +2436,14 @@
       <c r="H45" s="5">
         <v>5800000000</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I45" s="5">
+        <v>5800000000</v>
+      </c>
+      <c r="J45" s="5">
+        <v>5800000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>48</v>
       </c>
@@ -2198,8 +2468,14 @@
       <c r="H46" s="5">
         <v>25500000000</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I46" s="5">
+        <v>25500000000</v>
+      </c>
+      <c r="J46" s="5">
+        <v>25500000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>49</v>
       </c>
@@ -2224,8 +2500,14 @@
       <c r="H47" s="5">
         <v>20800000000</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I47" s="5">
+        <v>20800000000</v>
+      </c>
+      <c r="J47" s="5">
+        <v>20800000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>50</v>
       </c>
@@ -2250,8 +2532,14 @@
       <c r="H48" s="5">
         <v>42500000000</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I48" s="5">
+        <v>42500000000</v>
+      </c>
+      <c r="J48" s="5">
+        <v>42500000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>51</v>
       </c>
@@ -2276,8 +2564,14 @@
       <c r="H49" s="5">
         <v>39500000000</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I49" s="5">
+        <v>39500000000</v>
+      </c>
+      <c r="J49" s="5">
+        <v>39500000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>52</v>
       </c>
@@ -2302,8 +2596,14 @@
       <c r="H50" s="5">
         <v>29000000000</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I50" s="5">
+        <v>29000000000</v>
+      </c>
+      <c r="J50" s="5">
+        <v>29000000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>53</v>
       </c>
@@ -2328,8 +2628,14 @@
       <c r="H51" s="5">
         <v>15000000000</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I51" s="5">
+        <v>15000000000</v>
+      </c>
+      <c r="J51" s="5">
+        <v>15000000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>54</v>
       </c>
@@ -2354,8 +2660,14 @@
       <c r="H52" s="5">
         <v>19888000000</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I52" s="5">
+        <v>19888000000</v>
+      </c>
+      <c r="J52" s="5">
+        <v>19888000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>55</v>
       </c>
@@ -2380,8 +2692,14 @@
       <c r="H53" s="5">
         <v>32500000000</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I53" s="5">
+        <v>32500000000</v>
+      </c>
+      <c r="J53" s="5">
+        <v>32500000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>56</v>
       </c>
@@ -2406,8 +2724,14 @@
       <c r="H54" s="5">
         <v>365744000000</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I54" s="5">
+        <v>365744000000</v>
+      </c>
+      <c r="J54" s="5">
+        <v>365744000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>58</v>
       </c>
@@ -2432,8 +2756,14 @@
       <c r="H55" s="5">
         <v>74495000000</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I55" s="5">
+        <v>74495000000</v>
+      </c>
+      <c r="J55" s="5">
+        <v>74495000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>59</v>
       </c>
@@ -2458,8 +2788,14 @@
       <c r="H56" s="5">
         <v>114590000000</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I56" s="5">
+        <v>114590000000</v>
+      </c>
+      <c r="J56" s="5">
+        <v>114590000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>60</v>
       </c>
@@ -2484,8 +2820,14 @@
       <c r="H57" s="5">
         <v>23711000000</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I57" s="5">
+        <v>23711000000</v>
+      </c>
+      <c r="J57" s="5">
+        <v>23711000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>61</v>
       </c>
@@ -2510,8 +2852,14 @@
       <c r="H58" s="5">
         <v>19042000000</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I58" s="5">
+        <v>19042000000</v>
+      </c>
+      <c r="J58" s="5">
+        <v>19042000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>62</v>
       </c>
@@ -2536,8 +2884,14 @@
       <c r="H59" s="5">
         <v>21340000000</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I59" s="5">
+        <v>21340000000</v>
+      </c>
+      <c r="J59" s="5">
+        <v>21340000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>63</v>
       </c>
@@ -2562,8 +2916,14 @@
       <c r="H60" s="5">
         <v>8189000000</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I60" s="5">
+        <v>8189000000</v>
+      </c>
+      <c r="J60" s="5">
+        <v>8189000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>64</v>
       </c>
@@ -2588,8 +2948,14 @@
       <c r="H61" s="5">
         <v>56186000000</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I61" s="5">
+        <v>56186000000</v>
+      </c>
+      <c r="J61" s="5">
+        <v>56186000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>65</v>
       </c>
@@ -2614,8 +2980,14 @@
       <c r="H62" s="5">
         <v>16551000000</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I62" s="5">
+        <v>16551000000</v>
+      </c>
+      <c r="J62" s="5">
+        <v>16551000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>66</v>
       </c>
@@ -2640,8 +3012,14 @@
       <c r="H63" s="5">
         <v>14337000000</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I63" s="5">
+        <v>14337000000</v>
+      </c>
+      <c r="J63" s="5">
+        <v>14337000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>67</v>
       </c>
@@ -2666,8 +3044,14 @@
       <c r="H64" s="5">
         <v>17303000000</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I64" s="5">
+        <v>17303000000</v>
+      </c>
+      <c r="J64" s="5">
+        <v>17303000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>72</v>
       </c>
@@ -2692,8 +3076,14 @@
       <c r="H65" s="5">
         <v>281008000000</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I65" s="5">
+        <v>281008000000</v>
+      </c>
+      <c r="J65" s="5">
+        <v>281008000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>74</v>
       </c>
@@ -2718,8 +3108,14 @@
       <c r="H66" s="5">
         <v>19922502232</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I66" s="5">
+        <v>19922502232</v>
+      </c>
+      <c r="J66" s="5">
+        <v>19922502232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>75</v>
       </c>
@@ -2744,8 +3140,14 @@
       <c r="H67" s="5">
         <v>35884925597</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I67" s="5">
+        <v>35884925597</v>
+      </c>
+      <c r="J67" s="5">
+        <v>35884925597</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>76</v>
       </c>
@@ -2770,8 +3172,14 @@
       <c r="H68" s="5">
         <v>41962814799</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I68" s="5">
+        <v>41962814799</v>
+      </c>
+      <c r="J68" s="5">
+        <v>41962814799</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>77</v>
       </c>
@@ -2796,8 +3204,14 @@
       <c r="H69" s="5">
         <v>28610423344</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I69" s="5">
+        <v>28610423344</v>
+      </c>
+      <c r="J69" s="5">
+        <v>28610423344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>78</v>
       </c>
@@ -2822,8 +3236,14 @@
       <c r="H70" s="5">
         <v>11158550318</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I70" s="5">
+        <v>11158550318</v>
+      </c>
+      <c r="J70" s="5">
+        <v>11158550318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>79</v>
       </c>
@@ -2848,8 +3268,14 @@
       <c r="H71" s="5">
         <v>31893616813</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I71" s="5">
+        <v>31893616813</v>
+      </c>
+      <c r="J71" s="5">
+        <v>31893616813</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>80</v>
       </c>
@@ -2874,8 +3300,14 @@
       <c r="H72" s="5">
         <v>71324166334</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I72" s="5">
+        <v>71324166334</v>
+      </c>
+      <c r="J72" s="5">
+        <v>71324166334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>81</v>
       </c>
@@ -2900,8 +3332,14 @@
       <c r="H73" s="5">
         <v>21000116878</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I73" s="5">
+        <v>21000116878</v>
+      </c>
+      <c r="J73" s="5">
+        <v>21000116878</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>82</v>
       </c>
@@ -2926,8 +3364,14 @@
       <c r="H74" s="5">
         <v>13439081742</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I74" s="5">
+        <v>13439081742</v>
+      </c>
+      <c r="J74" s="5">
+        <v>13439081742</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>83</v>
       </c>
@@ -2952,8 +3396,14 @@
       <c r="H75" s="5">
         <v>5811801943</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I75" s="5">
+        <v>5811801943</v>
+      </c>
+      <c r="J75" s="5">
+        <v>5811801943</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>84</v>
       </c>
@@ -2978,8 +3428,14 @@
       <c r="H76" s="5">
         <v>266753000000</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I76" s="5">
+        <v>266753000000</v>
+      </c>
+      <c r="J76" s="5">
+        <v>266753000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>86</v>
       </c>
@@ -3004,8 +3460,14 @@
       <c r="H77" s="5">
         <v>60278000000</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I77" s="5">
+        <v>60278000000</v>
+      </c>
+      <c r="J77" s="5">
+        <v>60278000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>87</v>
       </c>
@@ -3030,8 +3492,14 @@
       <c r="H78" s="5">
         <v>20893000000</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I78" s="5">
+        <v>20893000000</v>
+      </c>
+      <c r="J78" s="5">
+        <v>20893000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>88</v>
       </c>
@@ -3056,8 +3524,14 @@
       <c r="H79" s="5">
         <v>35732000000</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I79" s="5">
+        <v>35732000000</v>
+      </c>
+      <c r="J79" s="5">
+        <v>35732000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>89</v>
       </c>
@@ -3082,8 +3556,14 @@
       <c r="H80" s="5">
         <v>73752000000</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I80" s="5">
+        <v>73752000000</v>
+      </c>
+      <c r="J80" s="5">
+        <v>73752000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>90</v>
       </c>
@@ -3108,8 +3588,14 @@
       <c r="H81" s="5">
         <v>8940000000</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I81" s="5">
+        <v>8940000000</v>
+      </c>
+      <c r="J81" s="5">
+        <v>8940000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>91</v>
       </c>
@@ -3134,8 +3620,14 @@
       <c r="H82" s="5">
         <v>11032000000</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I82" s="5">
+        <v>11032000000</v>
+      </c>
+      <c r="J82" s="5">
+        <v>11032000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>92</v>
       </c>
@@ -3160,8 +3652,14 @@
       <c r="H83" s="5">
         <v>23122000000</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I83" s="5">
+        <v>23122000000</v>
+      </c>
+      <c r="J83" s="5">
+        <v>23122000000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>93</v>
       </c>
@@ -3186,8 +3684,14 @@
       <c r="H84" s="5">
         <v>23550000000</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I84" s="5">
+        <v>23550000000</v>
+      </c>
+      <c r="J84" s="5">
+        <v>23550000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>94</v>
       </c>
@@ -3212,8 +3716,14 @@
       <c r="H85" s="5">
         <v>9454000000</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I85" s="5">
+        <v>9454000000</v>
+      </c>
+      <c r="J85" s="5">
+        <v>9454000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>97</v>
       </c>
@@ -3236,6 +3746,12 @@
         <v>210872531055</v>
       </c>
       <c r="H86" s="5">
+        <v>2826000000000</v>
+      </c>
+      <c r="I86" s="5">
+        <v>2826000000000</v>
+      </c>
+      <c r="J86" s="5">
         <v>2826000000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish layout and decentralization
</commit_message>
<xml_diff>
--- a/WebReport/WebReport/Content/upload/bao cao choi.xlsx
+++ b/WebReport/WebReport/Content/upload/bao cao choi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zawsz\OneDrive\Tài liệu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFD3CDD-AC92-4E33-AAF6-6A2AB8C3E439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA136CEC-287F-4021-8901-B3D800316912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D8E16A41-8E87-4CCF-B28E-281DB6006C9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D8E16A41-8E87-4CCF-B28E-281DB6006C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>TT</t>
   </si>
@@ -559,12 +567,6 @@
   </si>
   <si>
     <t>CHITIEU</t>
-  </si>
-  <si>
-    <t>TLQUY</t>
-  </si>
-  <si>
-    <t>TLNAM</t>
   </si>
 </sst>
 </file>
@@ -572,21 +574,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_)_$_ ;_ * \(#,##0\)_$_ ;_ * &quot;-&quot;??_)_$_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -651,7 +653,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -983,27 +985,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF96DBDC-24BE-4021-B36F-6A433E65D793}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20.25" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
+    <col min="6" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1020,22 +1020,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1060,14 +1054,8 @@
       <c r="H2" s="5">
         <v>0</v>
       </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1092,14 +1080,8 @@
       <c r="H3" s="5">
         <v>28897000000</v>
       </c>
-      <c r="I3" s="5">
-        <v>28897000000</v>
-      </c>
-      <c r="J3" s="5">
-        <v>28897000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1124,14 +1106,8 @@
       <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1156,14 +1132,8 @@
       <c r="H5" s="5">
         <v>20153000000</v>
       </c>
-      <c r="I5" s="5">
-        <v>20153000000</v>
-      </c>
-      <c r="J5" s="5">
-        <v>20153000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1188,14 +1158,8 @@
       <c r="H6" s="5">
         <v>8744000000</v>
       </c>
-      <c r="I6" s="5">
-        <v>8744000000</v>
-      </c>
-      <c r="J6" s="5">
-        <v>8744000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1220,14 +1184,8 @@
       <c r="H7" s="5">
         <v>14018000000</v>
       </c>
-      <c r="I7" s="5">
-        <v>14018000000</v>
-      </c>
-      <c r="J7" s="5">
-        <v>14018000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1252,14 +1210,8 @@
       <c r="H8" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -1284,14 +1236,8 @@
       <c r="H9" s="5">
         <v>14018000000</v>
       </c>
-      <c r="I9" s="5">
-        <v>14018000000</v>
-      </c>
-      <c r="J9" s="5">
-        <v>14018000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -1316,14 +1262,8 @@
       <c r="H10" s="5">
         <v>9988000000</v>
       </c>
-      <c r="I10" s="5">
-        <v>9988000000</v>
-      </c>
-      <c r="J10" s="5">
-        <v>9988000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -1348,14 +1288,8 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -1380,14 +1314,8 @@
       <c r="H12" s="5">
         <v>9988000000</v>
       </c>
-      <c r="I12" s="5">
-        <v>9988000000</v>
-      </c>
-      <c r="J12" s="5">
-        <v>9988000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -1412,14 +1340,8 @@
       <c r="H13" s="5">
         <v>8370000000</v>
       </c>
-      <c r="I13" s="5">
-        <v>8370000000</v>
-      </c>
-      <c r="J13" s="5">
-        <v>8370000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -1444,14 +1366,8 @@
       <c r="H14" s="5">
         <v>0</v>
       </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -1476,14 +1392,8 @@
       <c r="H15" s="5">
         <v>8370000000</v>
       </c>
-      <c r="I15" s="5">
-        <v>8370000000</v>
-      </c>
-      <c r="J15" s="5">
-        <v>8370000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1508,14 +1418,8 @@
       <c r="H16" s="5">
         <v>14200000000</v>
       </c>
-      <c r="I16" s="5">
-        <v>14200000000</v>
-      </c>
-      <c r="J16" s="5">
-        <v>14200000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1540,14 +1444,8 @@
       <c r="H17" s="5">
         <v>0</v>
       </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1572,14 +1470,8 @@
       <c r="H18" s="5">
         <v>10898000000</v>
       </c>
-      <c r="I18" s="5">
-        <v>10898000000</v>
-      </c>
-      <c r="J18" s="5">
-        <v>10898000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1604,14 +1496,8 @@
       <c r="H19" s="5">
         <v>3302000000</v>
       </c>
-      <c r="I19" s="5">
-        <v>3302000000</v>
-      </c>
-      <c r="J19" s="5">
-        <v>3302000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1636,14 +1522,8 @@
       <c r="H20" s="5">
         <v>12475000000</v>
       </c>
-      <c r="I20" s="5">
-        <v>12475000000</v>
-      </c>
-      <c r="J20" s="5">
-        <v>12475000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1668,14 +1548,8 @@
       <c r="H21" s="5">
         <v>0</v>
       </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1700,14 +1574,8 @@
       <c r="H22" s="5">
         <v>6453000000</v>
       </c>
-      <c r="I22" s="5">
-        <v>6453000000</v>
-      </c>
-      <c r="J22" s="5">
-        <v>6453000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1732,14 +1600,8 @@
       <c r="H23" s="5">
         <v>6022000000</v>
       </c>
-      <c r="I23" s="5">
-        <v>6022000000</v>
-      </c>
-      <c r="J23" s="5">
-        <v>6022000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1764,14 +1626,8 @@
       <c r="H24" s="5">
         <v>11363000000</v>
       </c>
-      <c r="I24" s="5">
-        <v>11363000000</v>
-      </c>
-      <c r="J24" s="5">
-        <v>11363000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1796,14 +1652,8 @@
       <c r="H25" s="5">
         <v>0</v>
       </c>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>26</v>
       </c>
@@ -1828,14 +1678,8 @@
       <c r="H26" s="5">
         <v>11363000000</v>
       </c>
-      <c r="I26" s="5">
-        <v>11363000000</v>
-      </c>
-      <c r="J26" s="5">
-        <v>11363000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1860,14 +1704,8 @@
       <c r="H27" s="5">
         <v>16600000000</v>
       </c>
-      <c r="I27" s="5">
-        <v>16600000000</v>
-      </c>
-      <c r="J27" s="5">
-        <v>16600000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1892,14 +1730,8 @@
       <c r="H28" s="5">
         <v>0</v>
       </c>
-      <c r="I28" s="5">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1924,14 +1756,8 @@
       <c r="H29" s="5">
         <v>9526000000</v>
       </c>
-      <c r="I29" s="5">
-        <v>9526000000</v>
-      </c>
-      <c r="J29" s="5">
-        <v>9526000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1956,14 +1782,8 @@
       <c r="H30" s="5">
         <v>7074000000</v>
       </c>
-      <c r="I30" s="5">
-        <v>7074000000</v>
-      </c>
-      <c r="J30" s="5">
-        <v>7074000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1988,14 +1808,8 @@
       <c r="H31" s="5">
         <v>13609000000</v>
       </c>
-      <c r="I31" s="5">
-        <v>13609000000</v>
-      </c>
-      <c r="J31" s="5">
-        <v>13609000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -2020,14 +1834,8 @@
       <c r="H32" s="5">
         <v>0</v>
       </c>
-      <c r="I32" s="5">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>33</v>
       </c>
@@ -2052,14 +1860,8 @@
       <c r="H33" s="5">
         <v>13609000000</v>
       </c>
-      <c r="I33" s="5">
-        <v>13609000000</v>
-      </c>
-      <c r="J33" s="5">
-        <v>13609000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>34</v>
       </c>
@@ -2084,14 +1886,8 @@
       <c r="H34" s="5">
         <v>9497000000</v>
       </c>
-      <c r="I34" s="5">
-        <v>9497000000</v>
-      </c>
-      <c r="J34" s="5">
-        <v>9497000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -2116,14 +1912,8 @@
       <c r="H35" s="5">
         <v>0</v>
       </c>
-      <c r="I35" s="5">
-        <v>0</v>
-      </c>
-      <c r="J35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -2148,14 +1938,8 @@
       <c r="H36" s="5">
         <v>9497000000</v>
       </c>
-      <c r="I36" s="5">
-        <v>9497000000</v>
-      </c>
-      <c r="J36" s="5">
-        <v>9497000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -2180,14 +1964,8 @@
       <c r="H37" s="5">
         <v>10590000000</v>
       </c>
-      <c r="I37" s="5">
-        <v>10590000000</v>
-      </c>
-      <c r="J37" s="5">
-        <v>10590000000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -2212,14 +1990,8 @@
       <c r="H38" s="5">
         <v>0</v>
       </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-      <c r="J38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>39</v>
       </c>
@@ -2244,14 +2016,8 @@
       <c r="H39" s="5">
         <v>5764000000</v>
       </c>
-      <c r="I39" s="5">
-        <v>5764000000</v>
-      </c>
-      <c r="J39" s="5">
-        <v>5764000000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>40</v>
       </c>
@@ -2276,14 +2042,8 @@
       <c r="H40" s="5">
         <v>4826000000</v>
       </c>
-      <c r="I40" s="5">
-        <v>4826000000</v>
-      </c>
-      <c r="J40" s="5">
-        <v>4826000000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -2308,14 +2068,8 @@
       <c r="H41" s="5">
         <v>1471700000000</v>
       </c>
-      <c r="I41" s="5">
-        <v>1471700000000</v>
-      </c>
-      <c r="J41" s="5">
-        <v>1471700000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>43</v>
       </c>
@@ -2340,14 +2094,8 @@
       <c r="H42" s="5">
         <v>291188000000</v>
       </c>
-      <c r="I42" s="5">
-        <v>291188000000</v>
-      </c>
-      <c r="J42" s="5">
-        <v>291188000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>45</v>
       </c>
@@ -2372,14 +2120,8 @@
       <c r="H43" s="5">
         <v>29700000000</v>
       </c>
-      <c r="I43" s="5">
-        <v>29700000000</v>
-      </c>
-      <c r="J43" s="5">
-        <v>29700000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>46</v>
       </c>
@@ -2404,14 +2146,8 @@
       <c r="H44" s="5">
         <v>31000000000</v>
       </c>
-      <c r="I44" s="5">
-        <v>31000000000</v>
-      </c>
-      <c r="J44" s="5">
-        <v>31000000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>47</v>
       </c>
@@ -2436,14 +2172,8 @@
       <c r="H45" s="5">
         <v>5800000000</v>
       </c>
-      <c r="I45" s="5">
-        <v>5800000000</v>
-      </c>
-      <c r="J45" s="5">
-        <v>5800000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>48</v>
       </c>
@@ -2468,14 +2198,8 @@
       <c r="H46" s="5">
         <v>25500000000</v>
       </c>
-      <c r="I46" s="5">
-        <v>25500000000</v>
-      </c>
-      <c r="J46" s="5">
-        <v>25500000000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>49</v>
       </c>
@@ -2500,14 +2224,8 @@
       <c r="H47" s="5">
         <v>20800000000</v>
       </c>
-      <c r="I47" s="5">
-        <v>20800000000</v>
-      </c>
-      <c r="J47" s="5">
-        <v>20800000000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>50</v>
       </c>
@@ -2532,14 +2250,8 @@
       <c r="H48" s="5">
         <v>42500000000</v>
       </c>
-      <c r="I48" s="5">
-        <v>42500000000</v>
-      </c>
-      <c r="J48" s="5">
-        <v>42500000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>51</v>
       </c>
@@ -2564,14 +2276,8 @@
       <c r="H49" s="5">
         <v>39500000000</v>
       </c>
-      <c r="I49" s="5">
-        <v>39500000000</v>
-      </c>
-      <c r="J49" s="5">
-        <v>39500000000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>52</v>
       </c>
@@ -2596,14 +2302,8 @@
       <c r="H50" s="5">
         <v>29000000000</v>
       </c>
-      <c r="I50" s="5">
-        <v>29000000000</v>
-      </c>
-      <c r="J50" s="5">
-        <v>29000000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>53</v>
       </c>
@@ -2628,14 +2328,8 @@
       <c r="H51" s="5">
         <v>15000000000</v>
       </c>
-      <c r="I51" s="5">
-        <v>15000000000</v>
-      </c>
-      <c r="J51" s="5">
-        <v>15000000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>54</v>
       </c>
@@ -2660,14 +2354,8 @@
       <c r="H52" s="5">
         <v>19888000000</v>
       </c>
-      <c r="I52" s="5">
-        <v>19888000000</v>
-      </c>
-      <c r="J52" s="5">
-        <v>19888000000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>55</v>
       </c>
@@ -2692,14 +2380,8 @@
       <c r="H53" s="5">
         <v>32500000000</v>
       </c>
-      <c r="I53" s="5">
-        <v>32500000000</v>
-      </c>
-      <c r="J53" s="5">
-        <v>32500000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>56</v>
       </c>
@@ -2724,14 +2406,8 @@
       <c r="H54" s="5">
         <v>365744000000</v>
       </c>
-      <c r="I54" s="5">
-        <v>365744000000</v>
-      </c>
-      <c r="J54" s="5">
-        <v>365744000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>58</v>
       </c>
@@ -2756,14 +2432,8 @@
       <c r="H55" s="5">
         <v>74495000000</v>
       </c>
-      <c r="I55" s="5">
-        <v>74495000000</v>
-      </c>
-      <c r="J55" s="5">
-        <v>74495000000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>59</v>
       </c>
@@ -2788,14 +2458,8 @@
       <c r="H56" s="5">
         <v>114590000000</v>
       </c>
-      <c r="I56" s="5">
-        <v>114590000000</v>
-      </c>
-      <c r="J56" s="5">
-        <v>114590000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>60</v>
       </c>
@@ -2820,14 +2484,8 @@
       <c r="H57" s="5">
         <v>23711000000</v>
       </c>
-      <c r="I57" s="5">
-        <v>23711000000</v>
-      </c>
-      <c r="J57" s="5">
-        <v>23711000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>61</v>
       </c>
@@ -2852,14 +2510,8 @@
       <c r="H58" s="5">
         <v>19042000000</v>
       </c>
-      <c r="I58" s="5">
-        <v>19042000000</v>
-      </c>
-      <c r="J58" s="5">
-        <v>19042000000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>62</v>
       </c>
@@ -2884,14 +2536,8 @@
       <c r="H59" s="5">
         <v>21340000000</v>
       </c>
-      <c r="I59" s="5">
-        <v>21340000000</v>
-      </c>
-      <c r="J59" s="5">
-        <v>21340000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>63</v>
       </c>
@@ -2916,14 +2562,8 @@
       <c r="H60" s="5">
         <v>8189000000</v>
       </c>
-      <c r="I60" s="5">
-        <v>8189000000</v>
-      </c>
-      <c r="J60" s="5">
-        <v>8189000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>64</v>
       </c>
@@ -2948,14 +2588,8 @@
       <c r="H61" s="5">
         <v>56186000000</v>
       </c>
-      <c r="I61" s="5">
-        <v>56186000000</v>
-      </c>
-      <c r="J61" s="5">
-        <v>56186000000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>65</v>
       </c>
@@ -2980,14 +2614,8 @@
       <c r="H62" s="5">
         <v>16551000000</v>
       </c>
-      <c r="I62" s="5">
-        <v>16551000000</v>
-      </c>
-      <c r="J62" s="5">
-        <v>16551000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>66</v>
       </c>
@@ -3012,14 +2640,8 @@
       <c r="H63" s="5">
         <v>14337000000</v>
       </c>
-      <c r="I63" s="5">
-        <v>14337000000</v>
-      </c>
-      <c r="J63" s="5">
-        <v>14337000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>67</v>
       </c>
@@ -3044,14 +2666,8 @@
       <c r="H64" s="5">
         <v>17303000000</v>
       </c>
-      <c r="I64" s="5">
-        <v>17303000000</v>
-      </c>
-      <c r="J64" s="5">
-        <v>17303000000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>72</v>
       </c>
@@ -3076,14 +2692,8 @@
       <c r="H65" s="5">
         <v>281008000000</v>
       </c>
-      <c r="I65" s="5">
-        <v>281008000000</v>
-      </c>
-      <c r="J65" s="5">
-        <v>281008000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>74</v>
       </c>
@@ -3108,14 +2718,8 @@
       <c r="H66" s="5">
         <v>19922502232</v>
       </c>
-      <c r="I66" s="5">
-        <v>19922502232</v>
-      </c>
-      <c r="J66" s="5">
-        <v>19922502232</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>75</v>
       </c>
@@ -3140,14 +2744,8 @@
       <c r="H67" s="5">
         <v>35884925597</v>
       </c>
-      <c r="I67" s="5">
-        <v>35884925597</v>
-      </c>
-      <c r="J67" s="5">
-        <v>35884925597</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>76</v>
       </c>
@@ -3172,14 +2770,8 @@
       <c r="H68" s="5">
         <v>41962814799</v>
       </c>
-      <c r="I68" s="5">
-        <v>41962814799</v>
-      </c>
-      <c r="J68" s="5">
-        <v>41962814799</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>77</v>
       </c>
@@ -3204,14 +2796,8 @@
       <c r="H69" s="5">
         <v>28610423344</v>
       </c>
-      <c r="I69" s="5">
-        <v>28610423344</v>
-      </c>
-      <c r="J69" s="5">
-        <v>28610423344</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>78</v>
       </c>
@@ -3236,14 +2822,8 @@
       <c r="H70" s="5">
         <v>11158550318</v>
       </c>
-      <c r="I70" s="5">
-        <v>11158550318</v>
-      </c>
-      <c r="J70" s="5">
-        <v>11158550318</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>79</v>
       </c>
@@ -3268,14 +2848,8 @@
       <c r="H71" s="5">
         <v>31893616813</v>
       </c>
-      <c r="I71" s="5">
-        <v>31893616813</v>
-      </c>
-      <c r="J71" s="5">
-        <v>31893616813</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>80</v>
       </c>
@@ -3300,14 +2874,8 @@
       <c r="H72" s="5">
         <v>71324166334</v>
       </c>
-      <c r="I72" s="5">
-        <v>71324166334</v>
-      </c>
-      <c r="J72" s="5">
-        <v>71324166334</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>81</v>
       </c>
@@ -3332,14 +2900,8 @@
       <c r="H73" s="5">
         <v>21000116878</v>
       </c>
-      <c r="I73" s="5">
-        <v>21000116878</v>
-      </c>
-      <c r="J73" s="5">
-        <v>21000116878</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>82</v>
       </c>
@@ -3364,14 +2926,8 @@
       <c r="H74" s="5">
         <v>13439081742</v>
       </c>
-      <c r="I74" s="5">
-        <v>13439081742</v>
-      </c>
-      <c r="J74" s="5">
-        <v>13439081742</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>83</v>
       </c>
@@ -3396,14 +2952,8 @@
       <c r="H75" s="5">
         <v>5811801943</v>
       </c>
-      <c r="I75" s="5">
-        <v>5811801943</v>
-      </c>
-      <c r="J75" s="5">
-        <v>5811801943</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>84</v>
       </c>
@@ -3428,14 +2978,8 @@
       <c r="H76" s="5">
         <v>266753000000</v>
       </c>
-      <c r="I76" s="5">
-        <v>266753000000</v>
-      </c>
-      <c r="J76" s="5">
-        <v>266753000000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>86</v>
       </c>
@@ -3460,14 +3004,8 @@
       <c r="H77" s="5">
         <v>60278000000</v>
       </c>
-      <c r="I77" s="5">
-        <v>60278000000</v>
-      </c>
-      <c r="J77" s="5">
-        <v>60278000000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>87</v>
       </c>
@@ -3492,14 +3030,8 @@
       <c r="H78" s="5">
         <v>20893000000</v>
       </c>
-      <c r="I78" s="5">
-        <v>20893000000</v>
-      </c>
-      <c r="J78" s="5">
-        <v>20893000000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>88</v>
       </c>
@@ -3524,14 +3056,8 @@
       <c r="H79" s="5">
         <v>35732000000</v>
       </c>
-      <c r="I79" s="5">
-        <v>35732000000</v>
-      </c>
-      <c r="J79" s="5">
-        <v>35732000000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>89</v>
       </c>
@@ -3556,14 +3082,8 @@
       <c r="H80" s="5">
         <v>73752000000</v>
       </c>
-      <c r="I80" s="5">
-        <v>73752000000</v>
-      </c>
-      <c r="J80" s="5">
-        <v>73752000000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>90</v>
       </c>
@@ -3588,14 +3108,8 @@
       <c r="H81" s="5">
         <v>8940000000</v>
       </c>
-      <c r="I81" s="5">
-        <v>8940000000</v>
-      </c>
-      <c r="J81" s="5">
-        <v>8940000000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>91</v>
       </c>
@@ -3620,14 +3134,8 @@
       <c r="H82" s="5">
         <v>11032000000</v>
       </c>
-      <c r="I82" s="5">
-        <v>11032000000</v>
-      </c>
-      <c r="J82" s="5">
-        <v>11032000000</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>92</v>
       </c>
@@ -3652,14 +3160,8 @@
       <c r="H83" s="5">
         <v>23122000000</v>
       </c>
-      <c r="I83" s="5">
-        <v>23122000000</v>
-      </c>
-      <c r="J83" s="5">
-        <v>23122000000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>93</v>
       </c>
@@ -3684,14 +3186,8 @@
       <c r="H84" s="5">
         <v>23550000000</v>
       </c>
-      <c r="I84" s="5">
-        <v>23550000000</v>
-      </c>
-      <c r="J84" s="5">
-        <v>23550000000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>94</v>
       </c>
@@ -3716,14 +3212,8 @@
       <c r="H85" s="5">
         <v>9454000000</v>
       </c>
-      <c r="I85" s="5">
-        <v>9454000000</v>
-      </c>
-      <c r="J85" s="5">
-        <v>9454000000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>97</v>
       </c>
@@ -3746,12 +3236,6 @@
         <v>210872531055</v>
       </c>
       <c r="H86" s="5">
-        <v>2826000000000</v>
-      </c>
-      <c r="I86" s="5">
-        <v>2826000000000</v>
-      </c>
-      <c r="J86" s="5">
         <v>2826000000000</v>
       </c>
     </row>

</xml_diff>